<commit_message>
Macc Elite leads template changes
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/PrintTemplateEliteNonRedeemedGifts.xlsx
+++ b/UDM.Insurance.Interface/Templates/PrintTemplateEliteNonRedeemedGifts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\udminsureAug2021\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5A2BA665-EA9C-4FA8-8F21-09A4B8776EF2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAC168B-8267-4E83-A54F-3112CDE8303F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="0" windowWidth="27795" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -45,6 +45,7 @@
     <definedName name="MaxCoverAmount" localSheetId="2">CoverAndLead!$BL$40</definedName>
     <definedName name="PhoneNumbers" localSheetId="2">CoverAndLead!$X$40</definedName>
     <definedName name="PostalCode" localSheetId="2">CoverAndLead!$AL$40</definedName>
+    <definedName name="Premarketed">CoverAndLead!$BI$44</definedName>
     <definedName name="Referror" localSheetId="2">CoverAndLead!$AZ$40</definedName>
     <definedName name="RefNo" localSheetId="2">CoverAndLead!$A$40</definedName>
     <definedName name="Relationship" localSheetId="2">CoverAndLead!$BE$40</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Campaign</t>
   </si>
@@ -235,6 +236,9 @@
   </si>
   <si>
     <t>Redeem Target</t>
+  </si>
+  <si>
+    <t>PM</t>
   </si>
 </sst>
 </file>
@@ -726,6 +730,102 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -762,101 +862,302 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -866,303 +1167,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1826,122 +1830,122 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="65"/>
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G4" s="6"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="53"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="53"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="53"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="42"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="44"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="34" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="41"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="48"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="51"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
@@ -2008,18 +2012,18 @@
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="51"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="38"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
@@ -2038,84 +2042,84 @@
       <c r="N23" s="1"/>
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52" t="s">
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="53"/>
-      <c r="G25" s="52" t="s">
+      <c r="F25" s="35"/>
+      <c r="G25" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="53"/>
-      <c r="I25" s="52" t="s">
+      <c r="H25" s="35"/>
+      <c r="I25" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="53"/>
-      <c r="K25" s="52" t="s">
+      <c r="J25" s="35"/>
+      <c r="K25" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="53"/>
-      <c r="M25" s="52" t="s">
+      <c r="L25" s="35"/>
+      <c r="M25" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N25" s="53"/>
+      <c r="N25" s="35"/>
     </row>
     <row r="26" spans="2:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="59">
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28">
         <v>0.12</v>
       </c>
-      <c r="H26" s="60"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="58"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="27"/>
       <c r="O26"/>
     </row>
     <row r="27" spans="2:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="54"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="59">
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28">
         <v>0.13</v>
       </c>
-      <c r="H27" s="60"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="58"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="27"/>
       <c r="O27"/>
     </row>
     <row r="28" spans="2:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="64">
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="32">
         <v>0.15</v>
       </c>
-      <c r="H28" s="64"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="63"/>
-      <c r="N28" s="63"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
       <c r="O28"/>
     </row>
     <row r="29" spans="2:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2123,6 +2127,38 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="E27:F27"/>
@@ -2135,38 +2171,6 @@
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="B16:K16"/>
-    <mergeCell ref="B22:K22"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2180,7 +2184,9 @@
   </sheetPr>
   <dimension ref="A1:BT45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BI44" sqref="BI44:BK45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3607,41 +3613,41 @@
       <c r="R21" s="16"/>
       <c r="S21" s="16"/>
       <c r="T21" s="16"/>
-      <c r="U21" s="86" t="s">
+      <c r="U21" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="V21" s="87"/>
-      <c r="W21" s="87"/>
-      <c r="X21" s="87"/>
-      <c r="Y21" s="87"/>
-      <c r="Z21" s="87"/>
-      <c r="AA21" s="87"/>
-      <c r="AB21" s="87"/>
-      <c r="AC21" s="87"/>
-      <c r="AD21" s="87"/>
-      <c r="AE21" s="87"/>
-      <c r="AF21" s="87"/>
-      <c r="AG21" s="88"/>
-      <c r="AH21" s="88"/>
-      <c r="AI21" s="88"/>
-      <c r="AJ21" s="88"/>
-      <c r="AK21" s="88"/>
-      <c r="AL21" s="88"/>
-      <c r="AM21" s="88"/>
-      <c r="AN21" s="88"/>
-      <c r="AO21" s="88"/>
-      <c r="AP21" s="88"/>
-      <c r="AQ21" s="88"/>
-      <c r="AR21" s="88"/>
-      <c r="AS21" s="88"/>
-      <c r="AT21" s="88"/>
-      <c r="AU21" s="88"/>
-      <c r="AV21" s="88"/>
-      <c r="AW21" s="88"/>
-      <c r="AX21" s="88"/>
-      <c r="AY21" s="88"/>
-      <c r="AZ21" s="88"/>
-      <c r="BA21" s="89"/>
+      <c r="V21" s="146"/>
+      <c r="W21" s="146"/>
+      <c r="X21" s="146"/>
+      <c r="Y21" s="146"/>
+      <c r="Z21" s="146"/>
+      <c r="AA21" s="146"/>
+      <c r="AB21" s="146"/>
+      <c r="AC21" s="146"/>
+      <c r="AD21" s="146"/>
+      <c r="AE21" s="146"/>
+      <c r="AF21" s="146"/>
+      <c r="AG21" s="147"/>
+      <c r="AH21" s="147"/>
+      <c r="AI21" s="147"/>
+      <c r="AJ21" s="147"/>
+      <c r="AK21" s="147"/>
+      <c r="AL21" s="147"/>
+      <c r="AM21" s="147"/>
+      <c r="AN21" s="147"/>
+      <c r="AO21" s="147"/>
+      <c r="AP21" s="147"/>
+      <c r="AQ21" s="147"/>
+      <c r="AR21" s="147"/>
+      <c r="AS21" s="147"/>
+      <c r="AT21" s="147"/>
+      <c r="AU21" s="147"/>
+      <c r="AV21" s="147"/>
+      <c r="AW21" s="147"/>
+      <c r="AX21" s="147"/>
+      <c r="AY21" s="147"/>
+      <c r="AZ21" s="147"/>
+      <c r="BA21" s="148"/>
       <c r="BB21" s="16"/>
       <c r="BC21" s="16"/>
       <c r="BD21" s="16"/>
@@ -3679,41 +3685,41 @@
       <c r="R22" s="16"/>
       <c r="S22" s="16"/>
       <c r="T22" s="16"/>
-      <c r="U22" s="84" t="s">
+      <c r="U22" s="143" t="s">
         <v>1</v>
       </c>
-      <c r="V22" s="85"/>
-      <c r="W22" s="85"/>
-      <c r="X22" s="85"/>
-      <c r="Y22" s="85"/>
-      <c r="Z22" s="85"/>
-      <c r="AA22" s="85"/>
-      <c r="AB22" s="85"/>
-      <c r="AC22" s="85"/>
-      <c r="AD22" s="85"/>
-      <c r="AE22" s="85"/>
-      <c r="AF22" s="85"/>
-      <c r="AG22" s="90"/>
-      <c r="AH22" s="90"/>
-      <c r="AI22" s="90"/>
-      <c r="AJ22" s="90"/>
-      <c r="AK22" s="90"/>
-      <c r="AL22" s="90"/>
-      <c r="AM22" s="90"/>
-      <c r="AN22" s="90"/>
-      <c r="AO22" s="90"/>
-      <c r="AP22" s="90"/>
-      <c r="AQ22" s="90"/>
-      <c r="AR22" s="90"/>
-      <c r="AS22" s="90"/>
-      <c r="AT22" s="90"/>
-      <c r="AU22" s="90"/>
-      <c r="AV22" s="90"/>
-      <c r="AW22" s="90"/>
-      <c r="AX22" s="90"/>
-      <c r="AY22" s="90"/>
-      <c r="AZ22" s="90"/>
-      <c r="BA22" s="91"/>
+      <c r="V22" s="144"/>
+      <c r="W22" s="144"/>
+      <c r="X22" s="144"/>
+      <c r="Y22" s="144"/>
+      <c r="Z22" s="144"/>
+      <c r="AA22" s="144"/>
+      <c r="AB22" s="144"/>
+      <c r="AC22" s="144"/>
+      <c r="AD22" s="144"/>
+      <c r="AE22" s="144"/>
+      <c r="AF22" s="144"/>
+      <c r="AG22" s="149"/>
+      <c r="AH22" s="149"/>
+      <c r="AI22" s="149"/>
+      <c r="AJ22" s="149"/>
+      <c r="AK22" s="149"/>
+      <c r="AL22" s="149"/>
+      <c r="AM22" s="149"/>
+      <c r="AN22" s="149"/>
+      <c r="AO22" s="149"/>
+      <c r="AP22" s="149"/>
+      <c r="AQ22" s="149"/>
+      <c r="AR22" s="149"/>
+      <c r="AS22" s="149"/>
+      <c r="AT22" s="149"/>
+      <c r="AU22" s="149"/>
+      <c r="AV22" s="149"/>
+      <c r="AW22" s="149"/>
+      <c r="AX22" s="149"/>
+      <c r="AY22" s="149"/>
+      <c r="AZ22" s="149"/>
+      <c r="BA22" s="150"/>
       <c r="BB22" s="16"/>
       <c r="BC22" s="16"/>
       <c r="BD22" s="16"/>
@@ -3751,41 +3757,41 @@
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
       <c r="T23" s="16"/>
-      <c r="U23" s="84" t="s">
+      <c r="U23" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="V23" s="85"/>
-      <c r="W23" s="85"/>
-      <c r="X23" s="85"/>
-      <c r="Y23" s="85"/>
-      <c r="Z23" s="85"/>
-      <c r="AA23" s="85"/>
-      <c r="AB23" s="85"/>
-      <c r="AC23" s="85"/>
-      <c r="AD23" s="85"/>
-      <c r="AE23" s="85"/>
-      <c r="AF23" s="85"/>
-      <c r="AG23" s="90"/>
-      <c r="AH23" s="90"/>
-      <c r="AI23" s="90"/>
-      <c r="AJ23" s="90"/>
-      <c r="AK23" s="90"/>
-      <c r="AL23" s="90"/>
-      <c r="AM23" s="90"/>
-      <c r="AN23" s="90"/>
-      <c r="AO23" s="90"/>
-      <c r="AP23" s="90"/>
-      <c r="AQ23" s="90"/>
-      <c r="AR23" s="90"/>
-      <c r="AS23" s="90"/>
-      <c r="AT23" s="90"/>
-      <c r="AU23" s="90"/>
-      <c r="AV23" s="90"/>
-      <c r="AW23" s="90"/>
-      <c r="AX23" s="90"/>
-      <c r="AY23" s="90"/>
-      <c r="AZ23" s="90"/>
-      <c r="BA23" s="91"/>
+      <c r="V23" s="144"/>
+      <c r="W23" s="144"/>
+      <c r="X23" s="144"/>
+      <c r="Y23" s="144"/>
+      <c r="Z23" s="144"/>
+      <c r="AA23" s="144"/>
+      <c r="AB23" s="144"/>
+      <c r="AC23" s="144"/>
+      <c r="AD23" s="144"/>
+      <c r="AE23" s="144"/>
+      <c r="AF23" s="144"/>
+      <c r="AG23" s="149"/>
+      <c r="AH23" s="149"/>
+      <c r="AI23" s="149"/>
+      <c r="AJ23" s="149"/>
+      <c r="AK23" s="149"/>
+      <c r="AL23" s="149"/>
+      <c r="AM23" s="149"/>
+      <c r="AN23" s="149"/>
+      <c r="AO23" s="149"/>
+      <c r="AP23" s="149"/>
+      <c r="AQ23" s="149"/>
+      <c r="AR23" s="149"/>
+      <c r="AS23" s="149"/>
+      <c r="AT23" s="149"/>
+      <c r="AU23" s="149"/>
+      <c r="AV23" s="149"/>
+      <c r="AW23" s="149"/>
+      <c r="AX23" s="149"/>
+      <c r="AY23" s="149"/>
+      <c r="AZ23" s="149"/>
+      <c r="BA23" s="150"/>
       <c r="BB23" s="16"/>
       <c r="BC23" s="16"/>
       <c r="BD23" s="16"/>
@@ -3823,41 +3829,41 @@
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
       <c r="T24" s="16"/>
-      <c r="U24" s="84" t="s">
+      <c r="U24" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="V24" s="85"/>
-      <c r="W24" s="85"/>
-      <c r="X24" s="85"/>
-      <c r="Y24" s="85"/>
-      <c r="Z24" s="85"/>
-      <c r="AA24" s="85"/>
-      <c r="AB24" s="85"/>
-      <c r="AC24" s="85"/>
-      <c r="AD24" s="85"/>
-      <c r="AE24" s="85"/>
-      <c r="AF24" s="85"/>
-      <c r="AG24" s="90"/>
-      <c r="AH24" s="90"/>
-      <c r="AI24" s="90"/>
-      <c r="AJ24" s="90"/>
-      <c r="AK24" s="90"/>
-      <c r="AL24" s="90"/>
-      <c r="AM24" s="90"/>
-      <c r="AN24" s="90"/>
-      <c r="AO24" s="90"/>
-      <c r="AP24" s="90"/>
-      <c r="AQ24" s="90"/>
-      <c r="AR24" s="90"/>
-      <c r="AS24" s="90"/>
-      <c r="AT24" s="90"/>
-      <c r="AU24" s="90"/>
-      <c r="AV24" s="90"/>
-      <c r="AW24" s="90"/>
-      <c r="AX24" s="90"/>
-      <c r="AY24" s="90"/>
-      <c r="AZ24" s="90"/>
-      <c r="BA24" s="91"/>
+      <c r="V24" s="144"/>
+      <c r="W24" s="144"/>
+      <c r="X24" s="144"/>
+      <c r="Y24" s="144"/>
+      <c r="Z24" s="144"/>
+      <c r="AA24" s="144"/>
+      <c r="AB24" s="144"/>
+      <c r="AC24" s="144"/>
+      <c r="AD24" s="144"/>
+      <c r="AE24" s="144"/>
+      <c r="AF24" s="144"/>
+      <c r="AG24" s="149"/>
+      <c r="AH24" s="149"/>
+      <c r="AI24" s="149"/>
+      <c r="AJ24" s="149"/>
+      <c r="AK24" s="149"/>
+      <c r="AL24" s="149"/>
+      <c r="AM24" s="149"/>
+      <c r="AN24" s="149"/>
+      <c r="AO24" s="149"/>
+      <c r="AP24" s="149"/>
+      <c r="AQ24" s="149"/>
+      <c r="AR24" s="149"/>
+      <c r="AS24" s="149"/>
+      <c r="AT24" s="149"/>
+      <c r="AU24" s="149"/>
+      <c r="AV24" s="149"/>
+      <c r="AW24" s="149"/>
+      <c r="AX24" s="149"/>
+      <c r="AY24" s="149"/>
+      <c r="AZ24" s="149"/>
+      <c r="BA24" s="150"/>
       <c r="BB24" s="16"/>
       <c r="BC24" s="16"/>
       <c r="BD24" s="16"/>
@@ -3895,41 +3901,41 @@
       <c r="R25" s="16"/>
       <c r="S25" s="16"/>
       <c r="T25" s="16"/>
-      <c r="U25" s="84" t="s">
+      <c r="U25" s="143" t="s">
         <v>4</v>
       </c>
-      <c r="V25" s="85"/>
-      <c r="W25" s="85"/>
-      <c r="X25" s="85"/>
-      <c r="Y25" s="85"/>
-      <c r="Z25" s="85"/>
-      <c r="AA25" s="85"/>
-      <c r="AB25" s="85"/>
-      <c r="AC25" s="85"/>
-      <c r="AD25" s="85"/>
-      <c r="AE25" s="85"/>
-      <c r="AF25" s="85"/>
-      <c r="AG25" s="92"/>
-      <c r="AH25" s="92"/>
-      <c r="AI25" s="92"/>
-      <c r="AJ25" s="92"/>
-      <c r="AK25" s="92"/>
-      <c r="AL25" s="92"/>
-      <c r="AM25" s="92"/>
-      <c r="AN25" s="92"/>
-      <c r="AO25" s="92"/>
-      <c r="AP25" s="92"/>
-      <c r="AQ25" s="92"/>
-      <c r="AR25" s="92"/>
-      <c r="AS25" s="92"/>
-      <c r="AT25" s="92"/>
-      <c r="AU25" s="92"/>
-      <c r="AV25" s="92"/>
-      <c r="AW25" s="92"/>
-      <c r="AX25" s="92"/>
-      <c r="AY25" s="92"/>
-      <c r="AZ25" s="92"/>
-      <c r="BA25" s="93"/>
+      <c r="V25" s="144"/>
+      <c r="W25" s="144"/>
+      <c r="X25" s="144"/>
+      <c r="Y25" s="144"/>
+      <c r="Z25" s="144"/>
+      <c r="AA25" s="144"/>
+      <c r="AB25" s="144"/>
+      <c r="AC25" s="144"/>
+      <c r="AD25" s="144"/>
+      <c r="AE25" s="144"/>
+      <c r="AF25" s="144"/>
+      <c r="AG25" s="151"/>
+      <c r="AH25" s="151"/>
+      <c r="AI25" s="151"/>
+      <c r="AJ25" s="151"/>
+      <c r="AK25" s="151"/>
+      <c r="AL25" s="151"/>
+      <c r="AM25" s="151"/>
+      <c r="AN25" s="151"/>
+      <c r="AO25" s="151"/>
+      <c r="AP25" s="151"/>
+      <c r="AQ25" s="151"/>
+      <c r="AR25" s="151"/>
+      <c r="AS25" s="151"/>
+      <c r="AT25" s="151"/>
+      <c r="AU25" s="151"/>
+      <c r="AV25" s="151"/>
+      <c r="AW25" s="151"/>
+      <c r="AX25" s="151"/>
+      <c r="AY25" s="151"/>
+      <c r="AZ25" s="151"/>
+      <c r="BA25" s="152"/>
       <c r="BB25" s="16"/>
       <c r="BC25" s="16"/>
       <c r="BD25" s="16"/>
@@ -3967,41 +3973,41 @@
       <c r="R26" s="16"/>
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
-      <c r="U26" s="84" t="s">
+      <c r="U26" s="143" t="s">
         <v>50</v>
       </c>
-      <c r="V26" s="85"/>
-      <c r="W26" s="85"/>
-      <c r="X26" s="85"/>
-      <c r="Y26" s="85"/>
-      <c r="Z26" s="85"/>
-      <c r="AA26" s="85"/>
-      <c r="AB26" s="85"/>
-      <c r="AC26" s="85"/>
-      <c r="AD26" s="85"/>
-      <c r="AE26" s="85"/>
-      <c r="AF26" s="85"/>
-      <c r="AG26" s="90"/>
-      <c r="AH26" s="90"/>
-      <c r="AI26" s="90"/>
-      <c r="AJ26" s="90"/>
-      <c r="AK26" s="90"/>
-      <c r="AL26" s="90"/>
-      <c r="AM26" s="90"/>
-      <c r="AN26" s="90"/>
-      <c r="AO26" s="90"/>
-      <c r="AP26" s="90"/>
-      <c r="AQ26" s="90"/>
-      <c r="AR26" s="90"/>
-      <c r="AS26" s="90"/>
-      <c r="AT26" s="90"/>
-      <c r="AU26" s="90"/>
-      <c r="AV26" s="90"/>
-      <c r="AW26" s="90"/>
-      <c r="AX26" s="90"/>
-      <c r="AY26" s="90"/>
-      <c r="AZ26" s="90"/>
-      <c r="BA26" s="91"/>
+      <c r="V26" s="144"/>
+      <c r="W26" s="144"/>
+      <c r="X26" s="144"/>
+      <c r="Y26" s="144"/>
+      <c r="Z26" s="144"/>
+      <c r="AA26" s="144"/>
+      <c r="AB26" s="144"/>
+      <c r="AC26" s="144"/>
+      <c r="AD26" s="144"/>
+      <c r="AE26" s="144"/>
+      <c r="AF26" s="144"/>
+      <c r="AG26" s="149"/>
+      <c r="AH26" s="149"/>
+      <c r="AI26" s="149"/>
+      <c r="AJ26" s="149"/>
+      <c r="AK26" s="149"/>
+      <c r="AL26" s="149"/>
+      <c r="AM26" s="149"/>
+      <c r="AN26" s="149"/>
+      <c r="AO26" s="149"/>
+      <c r="AP26" s="149"/>
+      <c r="AQ26" s="149"/>
+      <c r="AR26" s="149"/>
+      <c r="AS26" s="149"/>
+      <c r="AT26" s="149"/>
+      <c r="AU26" s="149"/>
+      <c r="AV26" s="149"/>
+      <c r="AW26" s="149"/>
+      <c r="AX26" s="149"/>
+      <c r="AY26" s="149"/>
+      <c r="AZ26" s="149"/>
+      <c r="BA26" s="150"/>
       <c r="BB26" s="16"/>
       <c r="BC26" s="16"/>
       <c r="BD26" s="16"/>
@@ -4039,41 +4045,41 @@
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
-      <c r="U27" s="84" t="s">
+      <c r="U27" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="V27" s="85"/>
-      <c r="W27" s="85"/>
-      <c r="X27" s="85"/>
-      <c r="Y27" s="85"/>
-      <c r="Z27" s="85"/>
-      <c r="AA27" s="85"/>
-      <c r="AB27" s="85"/>
-      <c r="AC27" s="85"/>
-      <c r="AD27" s="85"/>
-      <c r="AE27" s="85"/>
-      <c r="AF27" s="85"/>
-      <c r="AG27" s="90"/>
-      <c r="AH27" s="90"/>
-      <c r="AI27" s="90"/>
-      <c r="AJ27" s="90"/>
-      <c r="AK27" s="90"/>
-      <c r="AL27" s="90"/>
-      <c r="AM27" s="90"/>
-      <c r="AN27" s="90"/>
-      <c r="AO27" s="90"/>
-      <c r="AP27" s="90"/>
-      <c r="AQ27" s="90"/>
-      <c r="AR27" s="90"/>
-      <c r="AS27" s="90"/>
-      <c r="AT27" s="90"/>
-      <c r="AU27" s="90"/>
-      <c r="AV27" s="90"/>
-      <c r="AW27" s="90"/>
-      <c r="AX27" s="90"/>
-      <c r="AY27" s="90"/>
-      <c r="AZ27" s="90"/>
-      <c r="BA27" s="91"/>
+      <c r="V27" s="144"/>
+      <c r="W27" s="144"/>
+      <c r="X27" s="144"/>
+      <c r="Y27" s="144"/>
+      <c r="Z27" s="144"/>
+      <c r="AA27" s="144"/>
+      <c r="AB27" s="144"/>
+      <c r="AC27" s="144"/>
+      <c r="AD27" s="144"/>
+      <c r="AE27" s="144"/>
+      <c r="AF27" s="144"/>
+      <c r="AG27" s="149"/>
+      <c r="AH27" s="149"/>
+      <c r="AI27" s="149"/>
+      <c r="AJ27" s="149"/>
+      <c r="AK27" s="149"/>
+      <c r="AL27" s="149"/>
+      <c r="AM27" s="149"/>
+      <c r="AN27" s="149"/>
+      <c r="AO27" s="149"/>
+      <c r="AP27" s="149"/>
+      <c r="AQ27" s="149"/>
+      <c r="AR27" s="149"/>
+      <c r="AS27" s="149"/>
+      <c r="AT27" s="149"/>
+      <c r="AU27" s="149"/>
+      <c r="AV27" s="149"/>
+      <c r="AW27" s="149"/>
+      <c r="AX27" s="149"/>
+      <c r="AY27" s="149"/>
+      <c r="AZ27" s="149"/>
+      <c r="BA27" s="150"/>
       <c r="BB27" s="12"/>
       <c r="BC27" s="12"/>
       <c r="BD27" s="12"/>
@@ -4111,43 +4117,43 @@
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
-      <c r="U28" s="151" t="s">
+      <c r="U28" s="153" t="s">
         <v>57</v>
       </c>
-      <c r="V28" s="152"/>
-      <c r="W28" s="152"/>
-      <c r="X28" s="152"/>
-      <c r="Y28" s="152"/>
-      <c r="Z28" s="152"/>
-      <c r="AA28" s="152"/>
-      <c r="AB28" s="152"/>
-      <c r="AC28" s="152"/>
-      <c r="AD28" s="152"/>
-      <c r="AE28" s="152"/>
-      <c r="AF28" s="153"/>
-      <c r="AG28" s="157">
+      <c r="V28" s="154"/>
+      <c r="W28" s="154"/>
+      <c r="X28" s="154"/>
+      <c r="Y28" s="154"/>
+      <c r="Z28" s="154"/>
+      <c r="AA28" s="154"/>
+      <c r="AB28" s="154"/>
+      <c r="AC28" s="154"/>
+      <c r="AD28" s="154"/>
+      <c r="AE28" s="154"/>
+      <c r="AF28" s="155"/>
+      <c r="AG28" s="159">
         <v>16</v>
       </c>
-      <c r="AH28" s="158"/>
-      <c r="AI28" s="158"/>
-      <c r="AJ28" s="158"/>
-      <c r="AK28" s="158"/>
-      <c r="AL28" s="158"/>
-      <c r="AM28" s="158"/>
-      <c r="AN28" s="158"/>
-      <c r="AO28" s="158"/>
-      <c r="AP28" s="158"/>
-      <c r="AQ28" s="158"/>
-      <c r="AR28" s="158"/>
-      <c r="AS28" s="158"/>
-      <c r="AT28" s="158"/>
-      <c r="AU28" s="158"/>
-      <c r="AV28" s="158"/>
-      <c r="AW28" s="158"/>
-      <c r="AX28" s="158"/>
-      <c r="AY28" s="158"/>
-      <c r="AZ28" s="158"/>
-      <c r="BA28" s="159"/>
+      <c r="AH28" s="160"/>
+      <c r="AI28" s="160"/>
+      <c r="AJ28" s="160"/>
+      <c r="AK28" s="160"/>
+      <c r="AL28" s="160"/>
+      <c r="AM28" s="160"/>
+      <c r="AN28" s="160"/>
+      <c r="AO28" s="160"/>
+      <c r="AP28" s="160"/>
+      <c r="AQ28" s="160"/>
+      <c r="AR28" s="160"/>
+      <c r="AS28" s="160"/>
+      <c r="AT28" s="160"/>
+      <c r="AU28" s="160"/>
+      <c r="AV28" s="160"/>
+      <c r="AW28" s="160"/>
+      <c r="AX28" s="160"/>
+      <c r="AY28" s="160"/>
+      <c r="AZ28" s="160"/>
+      <c r="BA28" s="161"/>
       <c r="BB28" s="12"/>
       <c r="BC28" s="12"/>
       <c r="BD28" s="12"/>
@@ -4185,39 +4191,39 @@
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
-      <c r="U29" s="154"/>
-      <c r="V29" s="155"/>
-      <c r="W29" s="155"/>
-      <c r="X29" s="155"/>
-      <c r="Y29" s="155"/>
-      <c r="Z29" s="155"/>
-      <c r="AA29" s="155"/>
-      <c r="AB29" s="155"/>
-      <c r="AC29" s="155"/>
-      <c r="AD29" s="155"/>
-      <c r="AE29" s="155"/>
-      <c r="AF29" s="156"/>
-      <c r="AG29" s="160"/>
-      <c r="AH29" s="161"/>
-      <c r="AI29" s="161"/>
-      <c r="AJ29" s="161"/>
-      <c r="AK29" s="161"/>
-      <c r="AL29" s="161"/>
-      <c r="AM29" s="161"/>
-      <c r="AN29" s="161"/>
-      <c r="AO29" s="161"/>
-      <c r="AP29" s="161"/>
-      <c r="AQ29" s="161"/>
-      <c r="AR29" s="161"/>
-      <c r="AS29" s="161"/>
-      <c r="AT29" s="161"/>
-      <c r="AU29" s="161"/>
-      <c r="AV29" s="161"/>
-      <c r="AW29" s="161"/>
-      <c r="AX29" s="161"/>
-      <c r="AY29" s="161"/>
-      <c r="AZ29" s="161"/>
-      <c r="BA29" s="162"/>
+      <c r="U29" s="156"/>
+      <c r="V29" s="157"/>
+      <c r="W29" s="157"/>
+      <c r="X29" s="157"/>
+      <c r="Y29" s="157"/>
+      <c r="Z29" s="157"/>
+      <c r="AA29" s="157"/>
+      <c r="AB29" s="157"/>
+      <c r="AC29" s="157"/>
+      <c r="AD29" s="157"/>
+      <c r="AE29" s="157"/>
+      <c r="AF29" s="158"/>
+      <c r="AG29" s="162"/>
+      <c r="AH29" s="163"/>
+      <c r="AI29" s="163"/>
+      <c r="AJ29" s="163"/>
+      <c r="AK29" s="163"/>
+      <c r="AL29" s="163"/>
+      <c r="AM29" s="163"/>
+      <c r="AN29" s="163"/>
+      <c r="AO29" s="163"/>
+      <c r="AP29" s="163"/>
+      <c r="AQ29" s="163"/>
+      <c r="AR29" s="163"/>
+      <c r="AS29" s="163"/>
+      <c r="AT29" s="163"/>
+      <c r="AU29" s="163"/>
+      <c r="AV29" s="163"/>
+      <c r="AW29" s="163"/>
+      <c r="AX29" s="163"/>
+      <c r="AY29" s="163"/>
+      <c r="AZ29" s="163"/>
+      <c r="BA29" s="164"/>
       <c r="BB29" s="12"/>
       <c r="BC29" s="12"/>
       <c r="BD29" s="12"/>
@@ -4798,118 +4804,118 @@
     </row>
     <row r="38" spans="1:72" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:72" x14ac:dyDescent="0.2">
-      <c r="A39" s="97" t="s">
+      <c r="A39" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="97"/>
-      <c r="C39" s="97"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="98" t="s">
+      <c r="B39" s="74"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="99"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="100"/>
-      <c r="I39" s="97" t="s">
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="J39" s="97"/>
-      <c r="K39" s="97"/>
-      <c r="L39" s="97"/>
-      <c r="M39" s="97"/>
-      <c r="N39" s="98" t="s">
+      <c r="J39" s="74"/>
+      <c r="K39" s="74"/>
+      <c r="L39" s="74"/>
+      <c r="M39" s="74"/>
+      <c r="N39" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="O39" s="100"/>
-      <c r="P39" s="97" t="s">
+      <c r="O39" s="73"/>
+      <c r="P39" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="Q39" s="97"/>
-      <c r="R39" s="97"/>
-      <c r="S39" s="97"/>
-      <c r="T39" s="97" t="s">
+      <c r="Q39" s="74"/>
+      <c r="R39" s="74"/>
+      <c r="S39" s="74"/>
+      <c r="T39" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="U39" s="97"/>
-      <c r="V39" s="97"/>
-      <c r="W39" s="97"/>
-      <c r="X39" s="97" t="s">
+      <c r="U39" s="74"/>
+      <c r="V39" s="74"/>
+      <c r="W39" s="74"/>
+      <c r="X39" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="Y39" s="97"/>
-      <c r="Z39" s="97"/>
-      <c r="AA39" s="97"/>
-      <c r="AB39" s="97"/>
-      <c r="AC39" s="97"/>
-      <c r="AD39" s="98" t="s">
+      <c r="Y39" s="74"/>
+      <c r="Z39" s="74"/>
+      <c r="AA39" s="74"/>
+      <c r="AB39" s="74"/>
+      <c r="AC39" s="74"/>
+      <c r="AD39" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="AE39" s="99"/>
-      <c r="AF39" s="99"/>
-      <c r="AG39" s="99"/>
-      <c r="AH39" s="99"/>
-      <c r="AI39" s="99"/>
-      <c r="AJ39" s="99"/>
-      <c r="AK39" s="100"/>
-      <c r="AL39" s="97" t="s">
+      <c r="AE39" s="72"/>
+      <c r="AF39" s="72"/>
+      <c r="AG39" s="72"/>
+      <c r="AH39" s="72"/>
+      <c r="AI39" s="72"/>
+      <c r="AJ39" s="72"/>
+      <c r="AK39" s="73"/>
+      <c r="AL39" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="AM39" s="97"/>
-      <c r="AN39" s="97"/>
-      <c r="AO39" s="98" t="s">
+      <c r="AM39" s="74"/>
+      <c r="AN39" s="74"/>
+      <c r="AO39" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="AP39" s="99"/>
-      <c r="AQ39" s="99"/>
-      <c r="AR39" s="99"/>
-      <c r="AS39" s="99"/>
-      <c r="AT39" s="100"/>
-      <c r="AU39" s="97" t="s">
+      <c r="AP39" s="72"/>
+      <c r="AQ39" s="72"/>
+      <c r="AR39" s="72"/>
+      <c r="AS39" s="72"/>
+      <c r="AT39" s="73"/>
+      <c r="AU39" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="AV39" s="97"/>
-      <c r="AW39" s="97"/>
-      <c r="AX39" s="97"/>
-      <c r="AY39" s="97"/>
-      <c r="AZ39" s="97" t="s">
+      <c r="AV39" s="74"/>
+      <c r="AW39" s="74"/>
+      <c r="AX39" s="74"/>
+      <c r="AY39" s="74"/>
+      <c r="AZ39" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="BA39" s="97"/>
-      <c r="BB39" s="97"/>
-      <c r="BC39" s="97"/>
-      <c r="BD39" s="97"/>
-      <c r="BE39" s="97" t="s">
+      <c r="BA39" s="74"/>
+      <c r="BB39" s="74"/>
+      <c r="BC39" s="74"/>
+      <c r="BD39" s="74"/>
+      <c r="BE39" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="BF39" s="97"/>
-      <c r="BG39" s="97"/>
-      <c r="BH39" s="97"/>
-      <c r="BI39" s="97"/>
-      <c r="BJ39" s="97" t="s">
+      <c r="BF39" s="74"/>
+      <c r="BG39" s="74"/>
+      <c r="BH39" s="74"/>
+      <c r="BI39" s="74"/>
+      <c r="BJ39" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="BK39" s="97"/>
-      <c r="BL39" s="97" t="s">
+      <c r="BK39" s="74"/>
+      <c r="BL39" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="BM39" s="97"/>
-      <c r="BN39" s="97"/>
-      <c r="BO39" s="97"/>
-      <c r="BP39" s="97"/>
-      <c r="BQ39" s="97"/>
-      <c r="BR39" s="97"/>
-      <c r="BS39" s="97"/>
-      <c r="BT39" s="97"/>
+      <c r="BM39" s="74"/>
+      <c r="BN39" s="74"/>
+      <c r="BO39" s="74"/>
+      <c r="BP39" s="74"/>
+      <c r="BQ39" s="74"/>
+      <c r="BR39" s="74"/>
+      <c r="BS39" s="74"/>
+      <c r="BT39" s="74"/>
     </row>
     <row r="40" spans="1:72" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="75"/>
       <c r="B40" s="76"/>
       <c r="C40" s="76"/>
       <c r="D40" s="77"/>
-      <c r="E40" s="142"/>
-      <c r="F40" s="143"/>
-      <c r="G40" s="143"/>
-      <c r="H40" s="144"/>
+      <c r="E40" s="107"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="109"/>
       <c r="I40" s="75"/>
       <c r="J40" s="76"/>
       <c r="K40" s="76"/>
@@ -4925,12 +4931,12 @@
       <c r="U40" s="76"/>
       <c r="V40" s="76"/>
       <c r="W40" s="77"/>
-      <c r="X40" s="110"/>
-      <c r="Y40" s="111"/>
-      <c r="Z40" s="111"/>
-      <c r="AA40" s="111"/>
-      <c r="AB40" s="111"/>
-      <c r="AC40" s="112"/>
+      <c r="X40" s="125"/>
+      <c r="Y40" s="126"/>
+      <c r="Z40" s="126"/>
+      <c r="AA40" s="126"/>
+      <c r="AB40" s="126"/>
+      <c r="AC40" s="127"/>
       <c r="AD40" s="75"/>
       <c r="AE40" s="76"/>
       <c r="AF40" s="76"/>
@@ -4942,12 +4948,12 @@
       <c r="AL40" s="75"/>
       <c r="AM40" s="76"/>
       <c r="AN40" s="77"/>
-      <c r="AO40" s="119"/>
-      <c r="AP40" s="120"/>
-      <c r="AQ40" s="120"/>
-      <c r="AR40" s="120"/>
-      <c r="AS40" s="120"/>
-      <c r="AT40" s="121"/>
+      <c r="AO40" s="134"/>
+      <c r="AP40" s="135"/>
+      <c r="AQ40" s="135"/>
+      <c r="AR40" s="135"/>
+      <c r="AS40" s="135"/>
+      <c r="AT40" s="136"/>
       <c r="AU40" s="75"/>
       <c r="AV40" s="76"/>
       <c r="AW40" s="76"/>
@@ -4965,25 +4971,25 @@
       <c r="BI40" s="77"/>
       <c r="BJ40" s="75"/>
       <c r="BK40" s="77"/>
-      <c r="BL40" s="101"/>
-      <c r="BM40" s="102"/>
-      <c r="BN40" s="102"/>
-      <c r="BO40" s="102"/>
-      <c r="BP40" s="102"/>
-      <c r="BQ40" s="102"/>
-      <c r="BR40" s="102"/>
-      <c r="BS40" s="102"/>
-      <c r="BT40" s="103"/>
+      <c r="BL40" s="116"/>
+      <c r="BM40" s="117"/>
+      <c r="BN40" s="117"/>
+      <c r="BO40" s="117"/>
+      <c r="BP40" s="117"/>
+      <c r="BQ40" s="117"/>
+      <c r="BR40" s="117"/>
+      <c r="BS40" s="117"/>
+      <c r="BT40" s="118"/>
     </row>
     <row r="41" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A41" s="78"/>
       <c r="B41" s="79"/>
       <c r="C41" s="79"/>
       <c r="D41" s="80"/>
-      <c r="E41" s="145"/>
-      <c r="F41" s="146"/>
-      <c r="G41" s="146"/>
-      <c r="H41" s="147"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="112"/>
       <c r="I41" s="78"/>
       <c r="J41" s="79"/>
       <c r="K41" s="79"/>
@@ -4999,12 +5005,12 @@
       <c r="U41" s="79"/>
       <c r="V41" s="79"/>
       <c r="W41" s="80"/>
-      <c r="X41" s="113"/>
-      <c r="Y41" s="114"/>
-      <c r="Z41" s="114"/>
-      <c r="AA41" s="114"/>
-      <c r="AB41" s="114"/>
-      <c r="AC41" s="115"/>
+      <c r="X41" s="128"/>
+      <c r="Y41" s="129"/>
+      <c r="Z41" s="129"/>
+      <c r="AA41" s="129"/>
+      <c r="AB41" s="129"/>
+      <c r="AC41" s="130"/>
       <c r="AD41" s="78"/>
       <c r="AE41" s="79"/>
       <c r="AF41" s="79"/>
@@ -5016,12 +5022,12 @@
       <c r="AL41" s="78"/>
       <c r="AM41" s="79"/>
       <c r="AN41" s="80"/>
-      <c r="AO41" s="122"/>
-      <c r="AP41" s="123"/>
-      <c r="AQ41" s="123"/>
-      <c r="AR41" s="123"/>
-      <c r="AS41" s="123"/>
-      <c r="AT41" s="124"/>
+      <c r="AO41" s="137"/>
+      <c r="AP41" s="138"/>
+      <c r="AQ41" s="138"/>
+      <c r="AR41" s="138"/>
+      <c r="AS41" s="138"/>
+      <c r="AT41" s="139"/>
       <c r="AU41" s="78"/>
       <c r="AV41" s="79"/>
       <c r="AW41" s="79"/>
@@ -5039,25 +5045,25 @@
       <c r="BI41" s="80"/>
       <c r="BJ41" s="78"/>
       <c r="BK41" s="80"/>
-      <c r="BL41" s="104"/>
-      <c r="BM41" s="105"/>
-      <c r="BN41" s="105"/>
-      <c r="BO41" s="105"/>
-      <c r="BP41" s="105"/>
-      <c r="BQ41" s="105"/>
-      <c r="BR41" s="105"/>
-      <c r="BS41" s="105"/>
-      <c r="BT41" s="106"/>
+      <c r="BL41" s="119"/>
+      <c r="BM41" s="120"/>
+      <c r="BN41" s="120"/>
+      <c r="BO41" s="120"/>
+      <c r="BP41" s="120"/>
+      <c r="BQ41" s="120"/>
+      <c r="BR41" s="120"/>
+      <c r="BS41" s="120"/>
+      <c r="BT41" s="121"/>
     </row>
     <row r="42" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A42" s="81"/>
       <c r="B42" s="82"/>
       <c r="C42" s="82"/>
       <c r="D42" s="83"/>
-      <c r="E42" s="148"/>
-      <c r="F42" s="149"/>
-      <c r="G42" s="149"/>
-      <c r="H42" s="150"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="114"/>
+      <c r="G42" s="114"/>
+      <c r="H42" s="115"/>
       <c r="I42" s="81"/>
       <c r="J42" s="82"/>
       <c r="K42" s="82"/>
@@ -5073,12 +5079,12 @@
       <c r="U42" s="82"/>
       <c r="V42" s="82"/>
       <c r="W42" s="83"/>
-      <c r="X42" s="116"/>
-      <c r="Y42" s="117"/>
-      <c r="Z42" s="117"/>
-      <c r="AA42" s="117"/>
-      <c r="AB42" s="117"/>
-      <c r="AC42" s="118"/>
+      <c r="X42" s="131"/>
+      <c r="Y42" s="132"/>
+      <c r="Z42" s="132"/>
+      <c r="AA42" s="132"/>
+      <c r="AB42" s="132"/>
+      <c r="AC42" s="133"/>
       <c r="AD42" s="81"/>
       <c r="AE42" s="82"/>
       <c r="AF42" s="82"/>
@@ -5090,12 +5096,12 @@
       <c r="AL42" s="81"/>
       <c r="AM42" s="82"/>
       <c r="AN42" s="83"/>
-      <c r="AO42" s="125"/>
-      <c r="AP42" s="126"/>
-      <c r="AQ42" s="126"/>
-      <c r="AR42" s="126"/>
-      <c r="AS42" s="126"/>
-      <c r="AT42" s="127"/>
+      <c r="AO42" s="140"/>
+      <c r="AP42" s="141"/>
+      <c r="AQ42" s="141"/>
+      <c r="AR42" s="141"/>
+      <c r="AS42" s="141"/>
+      <c r="AT42" s="142"/>
       <c r="AU42" s="81"/>
       <c r="AV42" s="82"/>
       <c r="AW42" s="82"/>
@@ -5113,343 +5119,424 @@
       <c r="BI42" s="83"/>
       <c r="BJ42" s="81"/>
       <c r="BK42" s="83"/>
-      <c r="BL42" s="107"/>
-      <c r="BM42" s="108"/>
-      <c r="BN42" s="108"/>
-      <c r="BO42" s="108"/>
-      <c r="BP42" s="108"/>
-      <c r="BQ42" s="108"/>
-      <c r="BR42" s="108"/>
-      <c r="BS42" s="108"/>
-      <c r="BT42" s="109"/>
+      <c r="BL42" s="122"/>
+      <c r="BM42" s="123"/>
+      <c r="BN42" s="123"/>
+      <c r="BO42" s="123"/>
+      <c r="BP42" s="123"/>
+      <c r="BQ42" s="123"/>
+      <c r="BR42" s="123"/>
+      <c r="BS42" s="123"/>
+      <c r="BT42" s="124"/>
     </row>
     <row r="43" spans="1:72" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="128" t="s">
+      <c r="A43" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="129"/>
-      <c r="C43" s="72" t="s">
+      <c r="B43" s="89"/>
+      <c r="C43" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="128" t="s">
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="H43" s="165"/>
-      <c r="I43" s="165"/>
-      <c r="J43" s="165"/>
-      <c r="K43" s="129"/>
-      <c r="L43" s="166" t="s">
+      <c r="H43" s="88"/>
+      <c r="I43" s="88"/>
+      <c r="J43" s="88"/>
+      <c r="K43" s="89"/>
+      <c r="L43" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="M43" s="167"/>
-      <c r="N43" s="136" t="s">
+      <c r="M43" s="97"/>
+      <c r="N43" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="O43" s="137"/>
-      <c r="P43" s="138"/>
-      <c r="Q43" s="94"/>
-      <c r="R43" s="95"/>
-      <c r="S43" s="96"/>
-      <c r="T43" s="94"/>
-      <c r="U43" s="95"/>
-      <c r="V43" s="96"/>
-      <c r="W43" s="94"/>
-      <c r="X43" s="95"/>
-      <c r="Y43" s="96"/>
-      <c r="Z43" s="130" t="s">
+      <c r="O43" s="91"/>
+      <c r="P43" s="92"/>
+      <c r="Q43" s="84"/>
+      <c r="R43" s="85"/>
+      <c r="S43" s="86"/>
+      <c r="T43" s="84"/>
+      <c r="U43" s="85"/>
+      <c r="V43" s="86"/>
+      <c r="W43" s="84"/>
+      <c r="X43" s="85"/>
+      <c r="Y43" s="86"/>
+      <c r="Z43" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="AA43" s="131"/>
-      <c r="AB43" s="131"/>
-      <c r="AC43" s="132"/>
-      <c r="AD43" s="94"/>
-      <c r="AE43" s="95"/>
-      <c r="AF43" s="96"/>
-      <c r="AG43" s="94"/>
-      <c r="AH43" s="95"/>
-      <c r="AI43" s="96"/>
-      <c r="AJ43" s="94"/>
-      <c r="AK43" s="95"/>
-      <c r="AL43" s="96"/>
-      <c r="AM43" s="94"/>
-      <c r="AN43" s="95"/>
-      <c r="AO43" s="96"/>
-      <c r="AP43" s="94"/>
-      <c r="AQ43" s="95"/>
-      <c r="AR43" s="96"/>
-      <c r="AS43" s="136" t="s">
+      <c r="AA43" s="102"/>
+      <c r="AB43" s="102"/>
+      <c r="AC43" s="103"/>
+      <c r="AD43" s="84"/>
+      <c r="AE43" s="85"/>
+      <c r="AF43" s="86"/>
+      <c r="AG43" s="84"/>
+      <c r="AH43" s="85"/>
+      <c r="AI43" s="86"/>
+      <c r="AJ43" s="84"/>
+      <c r="AK43" s="85"/>
+      <c r="AL43" s="86"/>
+      <c r="AM43" s="84"/>
+      <c r="AN43" s="85"/>
+      <c r="AO43" s="86"/>
+      <c r="AP43" s="84"/>
+      <c r="AQ43" s="85"/>
+      <c r="AR43" s="86"/>
+      <c r="AS43" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="AT43" s="137"/>
-      <c r="AU43" s="137"/>
-      <c r="AV43" s="138"/>
-      <c r="AW43" s="94"/>
-      <c r="AX43" s="95"/>
-      <c r="AY43" s="96"/>
-      <c r="AZ43" s="94"/>
-      <c r="BA43" s="95"/>
-      <c r="BB43" s="96"/>
-      <c r="BC43" s="94"/>
-      <c r="BD43" s="95"/>
-      <c r="BE43" s="96"/>
-      <c r="BF43" s="94"/>
-      <c r="BG43" s="95"/>
-      <c r="BH43" s="96"/>
-      <c r="BI43" s="94"/>
-      <c r="BJ43" s="95"/>
-      <c r="BK43" s="96"/>
-      <c r="BL43" s="98" t="s">
+      <c r="AT43" s="91"/>
+      <c r="AU43" s="91"/>
+      <c r="AV43" s="92"/>
+      <c r="AW43" s="84"/>
+      <c r="AX43" s="85"/>
+      <c r="AY43" s="86"/>
+      <c r="AZ43" s="84"/>
+      <c r="BA43" s="85"/>
+      <c r="BB43" s="86"/>
+      <c r="BC43" s="84"/>
+      <c r="BD43" s="85"/>
+      <c r="BE43" s="86"/>
+      <c r="BF43" s="84"/>
+      <c r="BG43" s="85"/>
+      <c r="BH43" s="86"/>
+      <c r="BI43" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ43" s="72"/>
+      <c r="BK43" s="73"/>
+      <c r="BL43" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="BM43" s="99"/>
-      <c r="BN43" s="99"/>
-      <c r="BO43" s="99"/>
-      <c r="BP43" s="99"/>
-      <c r="BQ43" s="99"/>
-      <c r="BR43" s="99"/>
-      <c r="BS43" s="99"/>
-      <c r="BT43" s="100"/>
+      <c r="BM43" s="72"/>
+      <c r="BN43" s="72"/>
+      <c r="BO43" s="72"/>
+      <c r="BP43" s="72"/>
+      <c r="BQ43" s="72"/>
+      <c r="BR43" s="72"/>
+      <c r="BS43" s="72"/>
+      <c r="BT43" s="73"/>
     </row>
     <row r="44" spans="1:72" x14ac:dyDescent="0.2">
-      <c r="A44" s="128" t="s">
+      <c r="A44" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="129"/>
-      <c r="C44" s="72" t="s">
+      <c r="B44" s="89"/>
+      <c r="C44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="128"/>
-      <c r="H44" s="165"/>
-      <c r="I44" s="165"/>
-      <c r="J44" s="165"/>
-      <c r="K44" s="129"/>
-      <c r="L44" s="166"/>
-      <c r="M44" s="167"/>
-      <c r="N44" s="139"/>
-      <c r="O44" s="140"/>
-      <c r="P44" s="141"/>
-      <c r="Q44" s="72" t="s">
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="88"/>
+      <c r="I44" s="88"/>
+      <c r="J44" s="88"/>
+      <c r="K44" s="89"/>
+      <c r="L44" s="96"/>
+      <c r="M44" s="97"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="94"/>
+      <c r="P44" s="95"/>
+      <c r="Q44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="R44" s="73"/>
-      <c r="S44" s="74"/>
-      <c r="T44" s="72" t="s">
+      <c r="R44" s="69"/>
+      <c r="S44" s="70"/>
+      <c r="T44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="U44" s="73"/>
-      <c r="V44" s="74"/>
-      <c r="W44" s="72" t="s">
+      <c r="U44" s="69"/>
+      <c r="V44" s="70"/>
+      <c r="W44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="X44" s="73"/>
-      <c r="Y44" s="74"/>
-      <c r="Z44" s="133"/>
-      <c r="AA44" s="134"/>
-      <c r="AB44" s="134"/>
-      <c r="AC44" s="135"/>
-      <c r="AD44" s="72" t="s">
+      <c r="X44" s="69"/>
+      <c r="Y44" s="70"/>
+      <c r="Z44" s="104"/>
+      <c r="AA44" s="105"/>
+      <c r="AB44" s="105"/>
+      <c r="AC44" s="106"/>
+      <c r="AD44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AE44" s="73"/>
-      <c r="AF44" s="74"/>
-      <c r="AG44" s="72" t="s">
+      <c r="AE44" s="69"/>
+      <c r="AF44" s="70"/>
+      <c r="AG44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AH44" s="73"/>
-      <c r="AI44" s="74"/>
-      <c r="AJ44" s="72" t="s">
+      <c r="AH44" s="69"/>
+      <c r="AI44" s="70"/>
+      <c r="AJ44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AK44" s="73"/>
-      <c r="AL44" s="74"/>
-      <c r="AM44" s="72" t="s">
+      <c r="AK44" s="69"/>
+      <c r="AL44" s="70"/>
+      <c r="AM44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AN44" s="73"/>
-      <c r="AO44" s="74"/>
-      <c r="AP44" s="72" t="s">
+      <c r="AN44" s="69"/>
+      <c r="AO44" s="70"/>
+      <c r="AP44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AQ44" s="73"/>
-      <c r="AR44" s="74"/>
-      <c r="AS44" s="139"/>
-      <c r="AT44" s="140"/>
-      <c r="AU44" s="140"/>
-      <c r="AV44" s="141"/>
-      <c r="AW44" s="72" t="s">
+      <c r="AQ44" s="69"/>
+      <c r="AR44" s="70"/>
+      <c r="AS44" s="93"/>
+      <c r="AT44" s="94"/>
+      <c r="AU44" s="94"/>
+      <c r="AV44" s="95"/>
+      <c r="AW44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="AX44" s="73"/>
-      <c r="AY44" s="74"/>
-      <c r="AZ44" s="72" t="s">
+      <c r="AX44" s="69"/>
+      <c r="AY44" s="70"/>
+      <c r="AZ44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="BA44" s="73"/>
-      <c r="BB44" s="74"/>
-      <c r="BC44" s="72" t="s">
+      <c r="BA44" s="69"/>
+      <c r="BB44" s="70"/>
+      <c r="BC44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="BD44" s="73"/>
-      <c r="BE44" s="74"/>
-      <c r="BF44" s="72" t="s">
+      <c r="BD44" s="69"/>
+      <c r="BE44" s="70"/>
+      <c r="BF44" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="BG44" s="73"/>
-      <c r="BH44" s="74"/>
-      <c r="BI44" s="72" t="s">
-        <v>35</v>
-      </c>
-      <c r="BJ44" s="73"/>
-      <c r="BK44" s="74"/>
-      <c r="BL44" s="69" t="s">
+      <c r="BG44" s="69"/>
+      <c r="BH44" s="70"/>
+      <c r="BI44" s="75"/>
+      <c r="BJ44" s="76"/>
+      <c r="BK44" s="77"/>
+      <c r="BL44" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="BM44" s="70"/>
-      <c r="BN44" s="71"/>
-      <c r="BO44" s="69" t="s">
+      <c r="BM44" s="99"/>
+      <c r="BN44" s="100"/>
+      <c r="BO44" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="BP44" s="71"/>
-      <c r="BQ44" s="69" t="s">
+      <c r="BP44" s="100"/>
+      <c r="BQ44" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="BR44" s="71"/>
-      <c r="BS44" s="69" t="s">
+      <c r="BR44" s="100"/>
+      <c r="BS44" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="BT44" s="71"/>
+      <c r="BT44" s="100"/>
     </row>
     <row r="45" spans="1:72" x14ac:dyDescent="0.2">
-      <c r="A45" s="163" t="s">
+      <c r="A45" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="164"/>
-      <c r="C45" s="72" t="s">
+      <c r="B45" s="67"/>
+      <c r="C45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="72" t="s">
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="H45" s="73"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="72" t="s">
+      <c r="H45" s="69"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="K45" s="73"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="72" t="s">
+      <c r="K45" s="69"/>
+      <c r="L45" s="70"/>
+      <c r="M45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="N45" s="73"/>
-      <c r="O45" s="74"/>
-      <c r="P45" s="72" t="s">
+      <c r="N45" s="69"/>
+      <c r="O45" s="70"/>
+      <c r="P45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="Q45" s="73"/>
-      <c r="R45" s="74"/>
-      <c r="S45" s="72" t="s">
+      <c r="Q45" s="69"/>
+      <c r="R45" s="70"/>
+      <c r="S45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="T45" s="73"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="72" t="s">
+      <c r="T45" s="69"/>
+      <c r="U45" s="70"/>
+      <c r="V45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="W45" s="73"/>
-      <c r="X45" s="74"/>
-      <c r="Y45" s="72" t="s">
+      <c r="W45" s="69"/>
+      <c r="X45" s="70"/>
+      <c r="Y45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="Z45" s="73"/>
-      <c r="AA45" s="74"/>
-      <c r="AB45" s="72" t="s">
+      <c r="Z45" s="69"/>
+      <c r="AA45" s="70"/>
+      <c r="AB45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AC45" s="73"/>
-      <c r="AD45" s="74"/>
-      <c r="AE45" s="72" t="s">
+      <c r="AC45" s="69"/>
+      <c r="AD45" s="70"/>
+      <c r="AE45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AF45" s="73"/>
-      <c r="AG45" s="74"/>
-      <c r="AH45" s="72" t="s">
+      <c r="AF45" s="69"/>
+      <c r="AG45" s="70"/>
+      <c r="AH45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AI45" s="73"/>
-      <c r="AJ45" s="74"/>
-      <c r="AK45" s="72" t="s">
+      <c r="AI45" s="69"/>
+      <c r="AJ45" s="70"/>
+      <c r="AK45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AL45" s="73"/>
-      <c r="AM45" s="74"/>
-      <c r="AN45" s="72" t="s">
+      <c r="AL45" s="69"/>
+      <c r="AM45" s="70"/>
+      <c r="AN45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AO45" s="73"/>
-      <c r="AP45" s="74"/>
-      <c r="AQ45" s="72" t="s">
+      <c r="AO45" s="69"/>
+      <c r="AP45" s="70"/>
+      <c r="AQ45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AR45" s="73"/>
-      <c r="AS45" s="74"/>
-      <c r="AT45" s="72" t="s">
+      <c r="AR45" s="69"/>
+      <c r="AS45" s="70"/>
+      <c r="AT45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AU45" s="73"/>
-      <c r="AV45" s="74"/>
-      <c r="AW45" s="72" t="s">
+      <c r="AU45" s="69"/>
+      <c r="AV45" s="70"/>
+      <c r="AW45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="AX45" s="73"/>
-      <c r="AY45" s="74"/>
-      <c r="AZ45" s="72" t="s">
+      <c r="AX45" s="69"/>
+      <c r="AY45" s="70"/>
+      <c r="AZ45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="BA45" s="73"/>
-      <c r="BB45" s="74"/>
-      <c r="BC45" s="72" t="s">
+      <c r="BA45" s="69"/>
+      <c r="BB45" s="70"/>
+      <c r="BC45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="BD45" s="73"/>
-      <c r="BE45" s="74"/>
-      <c r="BF45" s="72" t="s">
+      <c r="BD45" s="69"/>
+      <c r="BE45" s="70"/>
+      <c r="BF45" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="BG45" s="73"/>
-      <c r="BH45" s="74"/>
-      <c r="BI45" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="BJ45" s="73"/>
-      <c r="BK45" s="74"/>
-      <c r="BL45" s="69" t="s">
+      <c r="BG45" s="69"/>
+      <c r="BH45" s="70"/>
+      <c r="BI45" s="81"/>
+      <c r="BJ45" s="82"/>
+      <c r="BK45" s="83"/>
+      <c r="BL45" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="BM45" s="70"/>
-      <c r="BN45" s="71"/>
-      <c r="BO45" s="66" t="s">
+      <c r="BM45" s="99"/>
+      <c r="BN45" s="100"/>
+      <c r="BO45" s="165" t="s">
         <v>55</v>
       </c>
-      <c r="BP45" s="67"/>
-      <c r="BQ45" s="67"/>
-      <c r="BR45" s="67"/>
-      <c r="BS45" s="67"/>
-      <c r="BT45" s="68"/>
+      <c r="BP45" s="166"/>
+      <c r="BQ45" s="166"/>
+      <c r="BR45" s="166"/>
+      <c r="BS45" s="166"/>
+      <c r="BT45" s="167"/>
     </row>
   </sheetData>
-  <mergeCells count="111">
-    <mergeCell ref="E40:H42"/>
+  <mergeCells count="110">
+    <mergeCell ref="AP44:AR44"/>
     <mergeCell ref="U28:AF29"/>
     <mergeCell ref="AG28:BA29"/>
+    <mergeCell ref="BO45:BT45"/>
+    <mergeCell ref="BL45:BN45"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="P45:R45"/>
+    <mergeCell ref="S45:U45"/>
+    <mergeCell ref="V45:X45"/>
+    <mergeCell ref="Y45:AA45"/>
+    <mergeCell ref="AB45:AD45"/>
+    <mergeCell ref="AE45:AG45"/>
+    <mergeCell ref="AH45:AJ45"/>
+    <mergeCell ref="AK45:AM45"/>
+    <mergeCell ref="AN45:AP45"/>
+    <mergeCell ref="AZ45:BB45"/>
+    <mergeCell ref="BC45:BE45"/>
+    <mergeCell ref="BF45:BH45"/>
+    <mergeCell ref="AQ45:AS45"/>
+    <mergeCell ref="AT45:AV45"/>
+    <mergeCell ref="AW45:AY45"/>
+    <mergeCell ref="BI44:BK45"/>
+    <mergeCell ref="U23:AF23"/>
+    <mergeCell ref="U22:AF22"/>
+    <mergeCell ref="U21:AF21"/>
+    <mergeCell ref="AG21:BA21"/>
+    <mergeCell ref="AG22:BA22"/>
+    <mergeCell ref="AG23:BA23"/>
+    <mergeCell ref="U27:AF27"/>
+    <mergeCell ref="U26:AF26"/>
+    <mergeCell ref="U25:AF25"/>
+    <mergeCell ref="U24:AF24"/>
+    <mergeCell ref="AG24:BA24"/>
+    <mergeCell ref="AG25:BA25"/>
+    <mergeCell ref="AG26:BA26"/>
+    <mergeCell ref="AG27:BA27"/>
+    <mergeCell ref="BI43:BK43"/>
+    <mergeCell ref="BJ40:BK42"/>
+    <mergeCell ref="BL40:BT42"/>
+    <mergeCell ref="AL40:AN42"/>
+    <mergeCell ref="X40:AC42"/>
+    <mergeCell ref="AD40:AK42"/>
+    <mergeCell ref="AO40:AT42"/>
+    <mergeCell ref="P40:S42"/>
+    <mergeCell ref="AU40:AY42"/>
+    <mergeCell ref="AZ40:BD42"/>
+    <mergeCell ref="BE40:BI42"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="BL39:BT39"/>
+    <mergeCell ref="BJ39:BK39"/>
+    <mergeCell ref="AD39:AK39"/>
+    <mergeCell ref="X39:AC39"/>
+    <mergeCell ref="AU39:AY39"/>
+    <mergeCell ref="AZ39:BD39"/>
+    <mergeCell ref="BE39:BI39"/>
+    <mergeCell ref="AL39:AN39"/>
+    <mergeCell ref="T39:W39"/>
+    <mergeCell ref="P39:S39"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="BF44:BH44"/>
+    <mergeCell ref="BL44:BN44"/>
+    <mergeCell ref="BL43:BT43"/>
+    <mergeCell ref="BO44:BP44"/>
+    <mergeCell ref="BQ44:BR44"/>
+    <mergeCell ref="BS44:BT44"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="T44:V44"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="Z43:AC44"/>
+    <mergeCell ref="AJ44:AL44"/>
+    <mergeCell ref="BC43:BE43"/>
+    <mergeCell ref="AS43:AV44"/>
+    <mergeCell ref="AW43:AY43"/>
+    <mergeCell ref="AZ43:BB43"/>
+    <mergeCell ref="AW44:AY44"/>
+    <mergeCell ref="AZ44:BB44"/>
+    <mergeCell ref="AM44:AO44"/>
+    <mergeCell ref="AD43:AF43"/>
+    <mergeCell ref="BC44:BE44"/>
+    <mergeCell ref="Q43:S43"/>
+    <mergeCell ref="BF43:BH43"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="AG44:AI44"/>
     <mergeCell ref="AO39:AT39"/>
@@ -5471,93 +5558,9 @@
     <mergeCell ref="AD44:AF44"/>
     <mergeCell ref="G43:K43"/>
     <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="P40:S42"/>
     <mergeCell ref="A40:D42"/>
     <mergeCell ref="T40:W42"/>
-    <mergeCell ref="BF44:BH44"/>
-    <mergeCell ref="BI44:BK44"/>
-    <mergeCell ref="BL44:BN44"/>
-    <mergeCell ref="BL43:BT43"/>
-    <mergeCell ref="BO44:BP44"/>
-    <mergeCell ref="BQ44:BR44"/>
-    <mergeCell ref="BS44:BT44"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="T44:V44"/>
-    <mergeCell ref="W44:Y44"/>
-    <mergeCell ref="Z43:AC44"/>
-    <mergeCell ref="AJ44:AL44"/>
-    <mergeCell ref="BC43:BE43"/>
-    <mergeCell ref="AS43:AV44"/>
-    <mergeCell ref="AW43:AY43"/>
-    <mergeCell ref="AZ43:BB43"/>
-    <mergeCell ref="AW44:AY44"/>
-    <mergeCell ref="AZ44:BB44"/>
-    <mergeCell ref="AM44:AO44"/>
-    <mergeCell ref="AP44:AR44"/>
-    <mergeCell ref="AD43:AF43"/>
-    <mergeCell ref="BC44:BE44"/>
-    <mergeCell ref="Q43:S43"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="BL39:BT39"/>
-    <mergeCell ref="BJ39:BK39"/>
-    <mergeCell ref="AD39:AK39"/>
-    <mergeCell ref="X39:AC39"/>
-    <mergeCell ref="AU39:AY39"/>
-    <mergeCell ref="AZ39:BD39"/>
-    <mergeCell ref="BE39:BI39"/>
-    <mergeCell ref="AL39:AN39"/>
-    <mergeCell ref="T39:W39"/>
-    <mergeCell ref="P39:S39"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="BF43:BH43"/>
-    <mergeCell ref="BI43:BK43"/>
-    <mergeCell ref="BJ40:BK42"/>
-    <mergeCell ref="BL40:BT42"/>
-    <mergeCell ref="AL40:AN42"/>
-    <mergeCell ref="X40:AC42"/>
-    <mergeCell ref="AD40:AK42"/>
-    <mergeCell ref="AO40:AT42"/>
-    <mergeCell ref="AU40:AY42"/>
-    <mergeCell ref="AZ40:BD42"/>
-    <mergeCell ref="BE40:BI42"/>
-    <mergeCell ref="U23:AF23"/>
-    <mergeCell ref="U22:AF22"/>
-    <mergeCell ref="U21:AF21"/>
-    <mergeCell ref="AG21:BA21"/>
-    <mergeCell ref="AG22:BA22"/>
-    <mergeCell ref="AG23:BA23"/>
-    <mergeCell ref="U27:AF27"/>
-    <mergeCell ref="U26:AF26"/>
-    <mergeCell ref="U25:AF25"/>
-    <mergeCell ref="U24:AF24"/>
-    <mergeCell ref="AG24:BA24"/>
-    <mergeCell ref="AG25:BA25"/>
-    <mergeCell ref="AG26:BA26"/>
-    <mergeCell ref="AG27:BA27"/>
-    <mergeCell ref="BO45:BT45"/>
-    <mergeCell ref="BL45:BN45"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="P45:R45"/>
-    <mergeCell ref="S45:U45"/>
-    <mergeCell ref="V45:X45"/>
-    <mergeCell ref="Y45:AA45"/>
-    <mergeCell ref="AB45:AD45"/>
-    <mergeCell ref="AE45:AG45"/>
-    <mergeCell ref="AH45:AJ45"/>
-    <mergeCell ref="AK45:AM45"/>
-    <mergeCell ref="AN45:AP45"/>
-    <mergeCell ref="AZ45:BB45"/>
-    <mergeCell ref="BC45:BE45"/>
-    <mergeCell ref="BF45:BH45"/>
-    <mergeCell ref="BI45:BK45"/>
-    <mergeCell ref="AQ45:AS45"/>
-    <mergeCell ref="AT45:AV45"/>
-    <mergeCell ref="AW45:AY45"/>
+    <mergeCell ref="E40:H42"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>